<commit_message>
Marseille imports motif 1752 et ajout année 1754
</commit_message>
<xml_diff>
--- a/excel_sources/Local/Marseille/Marseille imports 1752.xlsx
+++ b/excel_sources/Local/Marseille/Marseille imports 1752.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-440" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5987" uniqueCount="612">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5986" uniqueCount="612">
   <si>
     <t>Entré par</t>
   </si>
@@ -1308,9 +1308,6 @@
     <t>bœuf salé</t>
   </si>
   <si>
-    <t>chiffres illisibles</t>
-  </si>
-  <si>
     <t>bois de sandal</t>
   </si>
   <si>
@@ -1855,6 +1852,9 @@
   </si>
   <si>
     <t>mules et mulets mulets</t>
+  </si>
+  <si>
+    <t>erreur de calcul (prix modifié mais pas le total n'a pas été recalculé)</t>
   </si>
 </sst>
 </file>
@@ -2063,17 +2063,7 @@
     <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2433,8 +2423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U850"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A843" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F854" sqref="F854"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4195,7 +4185,7 @@
         <v>22</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="G30" s="9" t="s">
         <v>23</v>
@@ -4313,7 +4303,7 @@
         <v>22</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="G32" s="9" t="s">
         <v>23</v>
@@ -6738,7 +6728,7 @@
         <v>22</v>
       </c>
       <c r="F73" s="18" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="G73" s="9" t="s">
         <v>23</v>
@@ -6915,7 +6905,7 @@
         <v>22</v>
       </c>
       <c r="F76" s="18" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="G76" s="9" t="s">
         <v>23</v>
@@ -7387,7 +7377,7 @@
         <v>22</v>
       </c>
       <c r="F84" s="9" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="G84" s="9" t="s">
         <v>23</v>
@@ -9106,7 +9096,7 @@
         <v>22</v>
       </c>
       <c r="F113" s="18" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="G113" s="9" t="s">
         <v>23</v>
@@ -9147,7 +9137,7 @@
         <v>-0.50000000000727596</v>
       </c>
       <c r="U113" s="8" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="114" spans="1:21">
@@ -9285,7 +9275,7 @@
         <v>22</v>
       </c>
       <c r="F116" s="9" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="G116" s="9" t="s">
         <v>23</v>
@@ -9344,7 +9334,7 @@
         <v>22</v>
       </c>
       <c r="F117" s="9" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="G117" s="9" t="s">
         <v>23</v>
@@ -9462,7 +9452,7 @@
         <v>22</v>
       </c>
       <c r="F119" s="18" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="G119" s="9" t="s">
         <v>23</v>
@@ -10408,7 +10398,7 @@
         <v>22</v>
       </c>
       <c r="F135" s="18" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="G135" s="9" t="s">
         <v>23</v>
@@ -10644,7 +10634,7 @@
         <v>22</v>
       </c>
       <c r="F139" s="18" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="G139" s="9" t="s">
         <v>23</v>
@@ -11724,12 +11714,14 @@
       </c>
       <c r="K157" s="13"/>
       <c r="L157" s="13">
-        <v>2</v>
-      </c>
-      <c r="M157" s="27"/>
+        <v>1</v>
+      </c>
+      <c r="M157" s="27">
+        <v>6</v>
+      </c>
       <c r="N157" s="24">
         <f t="shared" si="12"/>
-        <v>0.1</v>
+        <v>7.5000000000000011E-2</v>
       </c>
       <c r="O157" s="14">
         <v>333</v>
@@ -11742,15 +11734,13 @@
       </c>
       <c r="S157" s="16">
         <f t="shared" si="11"/>
-        <v>445</v>
+        <v>333.75000000000006</v>
       </c>
       <c r="T157" s="16">
         <f t="shared" si="14"/>
-        <v>-112</v>
-      </c>
-      <c r="U157" s="8" t="s">
-        <v>429</v>
-      </c>
+        <v>-0.75000000000005684</v>
+      </c>
+      <c r="U157" s="8"/>
     </row>
     <row r="158" spans="1:21">
       <c r="A158" s="8" t="s">
@@ -11769,7 +11759,7 @@
         <v>22</v>
       </c>
       <c r="F158" s="9" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G158" s="9" t="s">
         <v>23</v>
@@ -13187,7 +13177,7 @@
         <v>22</v>
       </c>
       <c r="F182" s="9" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G182" s="9" t="s">
         <v>23</v>
@@ -13305,7 +13295,7 @@
         <v>22</v>
       </c>
       <c r="F184" s="9" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G184" s="9" t="s">
         <v>23</v>
@@ -13423,7 +13413,7 @@
         <v>22</v>
       </c>
       <c r="F186" s="9" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G186" s="9" t="s">
         <v>23</v>
@@ -14072,7 +14062,7 @@
         <v>22</v>
       </c>
       <c r="F197" s="9" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="G197" s="9" t="s">
         <v>23</v>
@@ -14131,7 +14121,7 @@
         <v>22</v>
       </c>
       <c r="F198" s="9" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="G198" s="9" t="s">
         <v>23</v>
@@ -14310,7 +14300,7 @@
         <v>22</v>
       </c>
       <c r="F201" s="9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="G201" s="9" t="s">
         <v>23</v>
@@ -14442,7 +14432,7 @@
         <v>800</v>
       </c>
       <c r="J203" s="12" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="K203" s="13"/>
       <c r="L203" s="13">
@@ -14666,7 +14656,7 @@
         <v>22</v>
       </c>
       <c r="F207" s="9" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G207" s="9" t="s">
         <v>23</v>
@@ -15551,7 +15541,7 @@
         <v>22</v>
       </c>
       <c r="F222" s="9" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G222" s="9" t="s">
         <v>23</v>
@@ -15907,7 +15897,7 @@
         <v>22</v>
       </c>
       <c r="F228" s="9" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G228" s="9" t="s">
         <v>23</v>
@@ -16733,7 +16723,7 @@
         <v>22</v>
       </c>
       <c r="F242" s="9" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="G242" s="9" t="s">
         <v>23</v>
@@ -16772,7 +16762,7 @@
         <v>6000</v>
       </c>
       <c r="U242" s="8" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="243" spans="1:21">
@@ -16851,7 +16841,7 @@
         <v>22</v>
       </c>
       <c r="F244" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="G244" s="9" t="s">
         <v>23</v>
@@ -16922,7 +16912,7 @@
         <v>1336</v>
       </c>
       <c r="J245" s="12" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="K245" s="13">
         <v>3</v>
@@ -17030,7 +17020,7 @@
         <v>22</v>
       </c>
       <c r="F247" s="9" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="G247" s="9" t="s">
         <v>23</v>
@@ -17502,7 +17492,7 @@
         <v>22</v>
       </c>
       <c r="F255" s="9" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="G255" s="9" t="s">
         <v>23</v>
@@ -17679,7 +17669,7 @@
         <v>22</v>
       </c>
       <c r="F258" s="9" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="G258" s="9" t="s">
         <v>23</v>
@@ -17740,7 +17730,7 @@
         <v>22</v>
       </c>
       <c r="F259" s="9" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G259" s="9" t="s">
         <v>23</v>
@@ -17976,7 +17966,7 @@
         <v>22</v>
       </c>
       <c r="F263" s="9" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G263" s="9" t="s">
         <v>23</v>
@@ -17988,7 +17978,7 @@
         <v>3</v>
       </c>
       <c r="J263" s="12" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="K263" s="13">
         <v>1</v>
@@ -18035,7 +18025,7 @@
         <v>22</v>
       </c>
       <c r="F264" s="9" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="G264" s="9" t="s">
         <v>23</v>
@@ -18153,7 +18143,7 @@
         <v>22</v>
       </c>
       <c r="F266" s="9" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="G266" s="9" t="s">
         <v>23</v>
@@ -18625,7 +18615,7 @@
         <v>22</v>
       </c>
       <c r="F274" s="9" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="G274" s="9" t="s">
         <v>23</v>
@@ -18861,7 +18851,7 @@
         <v>22</v>
       </c>
       <c r="F278" s="9" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G278" s="9" t="s">
         <v>23</v>
@@ -18920,7 +18910,7 @@
         <v>22</v>
       </c>
       <c r="F279" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="G279" s="9" t="s">
         <v>23</v>
@@ -19156,7 +19146,7 @@
         <v>22</v>
       </c>
       <c r="F283" s="9" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="G283" s="9" t="s">
         <v>23</v>
@@ -19333,7 +19323,7 @@
         <v>22</v>
       </c>
       <c r="F286" s="9" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="G286" s="9" t="s">
         <v>23</v>
@@ -19392,7 +19382,7 @@
         <v>22</v>
       </c>
       <c r="F287" s="9" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="G287" s="9" t="s">
         <v>23</v>
@@ -19510,7 +19500,7 @@
         <v>22</v>
       </c>
       <c r="F289" s="9" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G289" s="9" t="s">
         <v>23</v>
@@ -19569,7 +19559,7 @@
         <v>22</v>
       </c>
       <c r="F290" s="9" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="G290" s="9" t="s">
         <v>23</v>
@@ -19628,7 +19618,7 @@
         <v>22</v>
       </c>
       <c r="F291" s="9" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="G291" s="9" t="s">
         <v>23</v>
@@ -19746,7 +19736,7 @@
         <v>22</v>
       </c>
       <c r="F293" s="9" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G293" s="9" t="s">
         <v>23</v>
@@ -20218,7 +20208,7 @@
         <v>22</v>
       </c>
       <c r="F301" s="9" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="G301" s="9" t="s">
         <v>23</v>
@@ -20633,7 +20623,7 @@
         <v>22</v>
       </c>
       <c r="F308" s="9" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="G308" s="9" t="s">
         <v>23</v>
@@ -20930,7 +20920,7 @@
         <v>22</v>
       </c>
       <c r="F313" s="9" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="G313" s="9" t="s">
         <v>23</v>
@@ -20971,7 +20961,7 @@
         <v>0</v>
       </c>
       <c r="U313" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="314" spans="1:21">
@@ -21288,7 +21278,7 @@
         <v>22</v>
       </c>
       <c r="F319" s="9" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="G319" s="9" t="s">
         <v>23</v>
@@ -21406,7 +21396,7 @@
         <v>22</v>
       </c>
       <c r="F321" s="9" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="G321" s="9" t="s">
         <v>23</v>
@@ -21524,7 +21514,7 @@
         <v>22</v>
       </c>
       <c r="F323" s="9" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="G323" s="9" t="s">
         <v>23</v>
@@ -21642,7 +21632,7 @@
         <v>22</v>
       </c>
       <c r="F325" s="9" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="G325" s="9" t="s">
         <v>23</v>
@@ -21701,7 +21691,7 @@
         <v>22</v>
       </c>
       <c r="F326" s="9" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G326" s="9" t="s">
         <v>23</v>
@@ -21937,7 +21927,7 @@
         <v>22</v>
       </c>
       <c r="F330" s="9" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G330" s="9" t="s">
         <v>23</v>
@@ -22173,7 +22163,7 @@
         <v>22</v>
       </c>
       <c r="F334" s="9" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G334" s="9" t="s">
         <v>23</v>
@@ -22232,7 +22222,7 @@
         <v>22</v>
       </c>
       <c r="F335" s="9" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G335" s="9" t="s">
         <v>23</v>
@@ -22468,7 +22458,7 @@
         <v>22</v>
       </c>
       <c r="F339" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G339" s="9" t="s">
         <v>23</v>
@@ -22704,7 +22694,7 @@
         <v>22</v>
       </c>
       <c r="F343" s="9" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="G343" s="9" t="s">
         <v>23</v>
@@ -22775,7 +22765,7 @@
         <v>13.5</v>
       </c>
       <c r="J344" s="12" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="K344" s="13">
         <v>3</v>
@@ -22940,7 +22930,7 @@
         <v>22</v>
       </c>
       <c r="F347" s="18" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="G347" s="9" t="s">
         <v>23</v>
@@ -23471,7 +23461,7 @@
         <v>22</v>
       </c>
       <c r="F356" s="9" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G356" s="9" t="s">
         <v>23</v>
@@ -23589,7 +23579,7 @@
         <v>22</v>
       </c>
       <c r="F358" s="9" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G358" s="9" t="s">
         <v>23</v>
@@ -23689,7 +23679,7 @@
         <v>0</v>
       </c>
       <c r="U359" s="8" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="360" spans="1:21">
@@ -24063,7 +24053,7 @@
         <v>22</v>
       </c>
       <c r="F366" s="9" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="G366" s="9" t="s">
         <v>23</v>
@@ -24240,7 +24230,7 @@
         <v>22</v>
       </c>
       <c r="F369" s="9" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="G369" s="9" t="s">
         <v>23</v>
@@ -24714,7 +24704,7 @@
         <v>22</v>
       </c>
       <c r="F377" s="18" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="G377" s="9" t="s">
         <v>23</v>
@@ -24832,7 +24822,7 @@
         <v>22</v>
       </c>
       <c r="F379" s="18" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="G379" s="9" t="s">
         <v>23</v>
@@ -25070,7 +25060,7 @@
         <v>22</v>
       </c>
       <c r="F383" s="9" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="G383" s="9" t="s">
         <v>23</v>
@@ -25424,7 +25414,7 @@
         <v>22</v>
       </c>
       <c r="F389" s="9" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="G389" s="9" t="s">
         <v>23</v>
@@ -25601,7 +25591,7 @@
         <v>22</v>
       </c>
       <c r="F392" s="9" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="G392" s="9" t="s">
         <v>23</v>
@@ -25955,7 +25945,7 @@
         <v>22</v>
       </c>
       <c r="F398" s="9" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="G398" s="9" t="s">
         <v>23</v>
@@ -26132,7 +26122,7 @@
         <v>22</v>
       </c>
       <c r="F401" s="9" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G401" s="9" t="s">
         <v>23</v>
@@ -26486,7 +26476,7 @@
         <v>22</v>
       </c>
       <c r="F407" s="9" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G407" s="9" t="s">
         <v>23</v>
@@ -26545,7 +26535,7 @@
         <v>22</v>
       </c>
       <c r="F408" s="9" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="G408" s="9" t="s">
         <v>23</v>
@@ -26604,7 +26594,7 @@
         <v>22</v>
       </c>
       <c r="F409" s="9" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="G409" s="9" t="s">
         <v>23</v>
@@ -26899,7 +26889,7 @@
         <v>22</v>
       </c>
       <c r="F414" s="9" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G414" s="9" t="s">
         <v>23</v>
@@ -26958,7 +26948,7 @@
         <v>22</v>
       </c>
       <c r="F415" s="9" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="G415" s="9" t="s">
         <v>23</v>
@@ -27136,7 +27126,7 @@
         <v>22</v>
       </c>
       <c r="F418" s="9" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="G418" s="9" t="s">
         <v>23</v>
@@ -27254,7 +27244,7 @@
         <v>22</v>
       </c>
       <c r="F420" s="9" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G420" s="9" t="s">
         <v>23</v>
@@ -27907,7 +27897,7 @@
         <v>22</v>
       </c>
       <c r="F431" s="9" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G431" s="9" t="s">
         <v>23</v>
@@ -28497,7 +28487,7 @@
         <v>22</v>
       </c>
       <c r="F441" s="9" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="G441" s="9" t="s">
         <v>23</v>
@@ -28615,7 +28605,7 @@
         <v>22</v>
       </c>
       <c r="F443" s="9" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="G443" s="9" t="s">
         <v>23</v>
@@ -28910,7 +28900,7 @@
         <v>22</v>
       </c>
       <c r="F448" s="9" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="G448" s="9" t="s">
         <v>23</v>
@@ -28969,7 +28959,7 @@
         <v>22</v>
       </c>
       <c r="F449" s="9" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="G449" s="9" t="s">
         <v>23</v>
@@ -29217,7 +29207,7 @@
         <v>2191</v>
       </c>
       <c r="J453" s="12" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="K453" s="13"/>
       <c r="L453" s="13">
@@ -29276,7 +29266,7 @@
         <v>212</v>
       </c>
       <c r="J454" s="12" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="K454" s="13">
         <v>30</v>
@@ -29382,7 +29372,7 @@
         <v>22</v>
       </c>
       <c r="F456" s="9" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="G456" s="9" t="s">
         <v>23</v>
@@ -29421,7 +29411,7 @@
         <v>20</v>
       </c>
       <c r="U456" s="8" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="457" spans="1:21">
@@ -29681,7 +29671,7 @@
         <v>22</v>
       </c>
       <c r="F461" s="9" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="G461" s="9" t="s">
         <v>23</v>
@@ -29740,7 +29730,7 @@
         <v>22</v>
       </c>
       <c r="F462" s="9" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="G462" s="9" t="s">
         <v>23</v>
@@ -30035,7 +30025,7 @@
         <v>22</v>
       </c>
       <c r="F467" s="26" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="G467" s="9" t="s">
         <v>23</v>
@@ -30094,7 +30084,7 @@
         <v>22</v>
       </c>
       <c r="F468" s="9" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="G468" s="9" t="s">
         <v>23</v>
@@ -30271,7 +30261,7 @@
         <v>22</v>
       </c>
       <c r="F471" s="9" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="G471" s="9" t="s">
         <v>23</v>
@@ -30389,7 +30379,7 @@
         <v>22</v>
       </c>
       <c r="F473" s="9" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G473" s="9" t="s">
         <v>23</v>
@@ -30448,7 +30438,7 @@
         <v>22</v>
       </c>
       <c r="F474" s="9" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="G474" s="9" t="s">
         <v>23</v>
@@ -30625,7 +30615,7 @@
         <v>22</v>
       </c>
       <c r="F477" s="9" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="G477" s="9" t="s">
         <v>23</v>
@@ -31510,7 +31500,7 @@
         <v>22</v>
       </c>
       <c r="F492" s="9" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G492" s="9" t="s">
         <v>23</v>
@@ -31569,7 +31559,7 @@
         <v>22</v>
       </c>
       <c r="F493" s="9" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="G493" s="9" t="s">
         <v>23</v>
@@ -31687,7 +31677,7 @@
         <v>22</v>
       </c>
       <c r="F495" s="9" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G495" s="9" t="s">
         <v>23</v>
@@ -31746,7 +31736,7 @@
         <v>22</v>
       </c>
       <c r="F496" s="9" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G496" s="9" t="s">
         <v>23</v>
@@ -32041,7 +32031,7 @@
         <v>22</v>
       </c>
       <c r="F501" s="9" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="G501" s="9" t="s">
         <v>23</v>
@@ -32159,7 +32149,7 @@
         <v>22</v>
       </c>
       <c r="F503" s="9" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="G503" s="9" t="s">
         <v>23</v>
@@ -32395,7 +32385,7 @@
         <v>22</v>
       </c>
       <c r="F507" s="9" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G507" s="9" t="s">
         <v>23</v>
@@ -32454,7 +32444,7 @@
         <v>22</v>
       </c>
       <c r="F508" s="9" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G508" s="9" t="s">
         <v>23</v>
@@ -32513,7 +32503,7 @@
         <v>22</v>
       </c>
       <c r="F509" s="9" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="G509" s="9" t="s">
         <v>23</v>
@@ -32631,7 +32621,7 @@
         <v>22</v>
       </c>
       <c r="F511" s="9" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G511" s="9" t="s">
         <v>23</v>
@@ -32690,7 +32680,7 @@
         <v>22</v>
       </c>
       <c r="F512" s="9" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="G512" s="9" t="s">
         <v>23</v>
@@ -33221,7 +33211,7 @@
         <v>22</v>
       </c>
       <c r="F521" s="9" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G521" s="9" t="s">
         <v>23</v>
@@ -33280,7 +33270,7 @@
         <v>22</v>
       </c>
       <c r="F522" s="9" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="G522" s="9" t="s">
         <v>23</v>
@@ -33457,7 +33447,7 @@
         <v>22</v>
       </c>
       <c r="F525" s="9" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G525" s="9" t="s">
         <v>23</v>
@@ -33516,7 +33506,7 @@
         <v>22</v>
       </c>
       <c r="F526" s="9" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="G526" s="9" t="s">
         <v>23</v>
@@ -33634,7 +33624,7 @@
         <v>22</v>
       </c>
       <c r="F528" s="9" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G528" s="9" t="s">
         <v>23</v>
@@ -34047,7 +34037,7 @@
         <v>22</v>
       </c>
       <c r="F535" s="9" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G535" s="9" t="s">
         <v>23</v>
@@ -34401,7 +34391,7 @@
         <v>22</v>
       </c>
       <c r="F541" s="9" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="G541" s="9" t="s">
         <v>23</v>
@@ -34757,7 +34747,7 @@
         <v>22</v>
       </c>
       <c r="F547" s="9" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G547" s="9" t="s">
         <v>23</v>
@@ -34993,7 +34983,7 @@
         <v>22</v>
       </c>
       <c r="F551" s="9" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G551" s="9" t="s">
         <v>23</v>
@@ -35229,7 +35219,7 @@
         <v>22</v>
       </c>
       <c r="F555" s="9" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="G555" s="9" t="s">
         <v>23</v>
@@ -35524,7 +35514,7 @@
         <v>22</v>
       </c>
       <c r="F560" s="9" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="G560" s="9" t="s">
         <v>23</v>
@@ -36118,7 +36108,7 @@
         <v>22</v>
       </c>
       <c r="F570" s="9" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="G570" s="9" t="s">
         <v>23</v>
@@ -36177,7 +36167,7 @@
         <v>22</v>
       </c>
       <c r="F571" s="9" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="G571" s="9" t="s">
         <v>23</v>
@@ -36295,7 +36285,7 @@
         <v>22</v>
       </c>
       <c r="F573" s="9" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="G573" s="9" t="s">
         <v>23</v>
@@ -36354,7 +36344,7 @@
         <v>22</v>
       </c>
       <c r="F574" s="18" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="G574" s="9" t="s">
         <v>23</v>
@@ -36590,7 +36580,7 @@
         <v>22</v>
       </c>
       <c r="F578" s="18" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="G578" s="9" t="s">
         <v>23</v>
@@ -36649,7 +36639,7 @@
         <v>22</v>
       </c>
       <c r="F579" s="18" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="G579" s="9" t="s">
         <v>23</v>
@@ -37182,7 +37172,7 @@
         <v>22</v>
       </c>
       <c r="F588" s="9" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="G588" s="9" t="s">
         <v>23</v>
@@ -37536,7 +37526,7 @@
         <v>22</v>
       </c>
       <c r="F594" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="G594" s="9" t="s">
         <v>23</v>
@@ -37595,7 +37585,7 @@
         <v>22</v>
       </c>
       <c r="F595" s="9" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="G595" s="9" t="s">
         <v>23</v>
@@ -37654,7 +37644,7 @@
         <v>22</v>
       </c>
       <c r="F596" s="9" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="G596" s="9" t="s">
         <v>23</v>
@@ -37772,7 +37762,7 @@
         <v>22</v>
       </c>
       <c r="F598" s="9" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="G598" s="9" t="s">
         <v>23</v>
@@ -38008,7 +37998,7 @@
         <v>22</v>
       </c>
       <c r="F602" s="9" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="G602" s="9" t="s">
         <v>23</v>
@@ -38244,7 +38234,7 @@
         <v>22</v>
       </c>
       <c r="F606" s="9" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="G606" s="9" t="s">
         <v>23</v>
@@ -38303,7 +38293,7 @@
         <v>22</v>
       </c>
       <c r="F607" s="9" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="G607" s="9" t="s">
         <v>23</v>
@@ -39011,7 +39001,7 @@
         <v>22</v>
       </c>
       <c r="F619" s="18" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="G619" s="9" t="s">
         <v>23</v>
@@ -39070,7 +39060,7 @@
         <v>22</v>
       </c>
       <c r="F620" s="18" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="G620" s="9" t="s">
         <v>23</v>
@@ -39778,7 +39768,7 @@
         <v>22</v>
       </c>
       <c r="F632" s="9" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="G632" s="9" t="s">
         <v>23</v>
@@ -40132,7 +40122,7 @@
         <v>22</v>
       </c>
       <c r="F638" s="9" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="G638" s="9" t="s">
         <v>23</v>
@@ -40291,7 +40281,7 @@
         <v>0</v>
       </c>
       <c r="U640" s="8" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="641" spans="1:21">
@@ -40901,7 +40891,7 @@
         <v>22</v>
       </c>
       <c r="F651" s="9" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G651" s="9" t="s">
         <v>23</v>
@@ -41078,7 +41068,7 @@
         <v>22</v>
       </c>
       <c r="F654" s="9" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="G654" s="9" t="s">
         <v>23</v>
@@ -41196,7 +41186,7 @@
         <v>22</v>
       </c>
       <c r="F656" s="9" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="G656" s="9" t="s">
         <v>23</v>
@@ -41491,7 +41481,7 @@
         <v>22</v>
       </c>
       <c r="F661" s="9" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="G661" s="9" t="s">
         <v>23</v>
@@ -41609,7 +41599,7 @@
         <v>22</v>
       </c>
       <c r="F663" s="9" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="G663" s="9" t="s">
         <v>23</v>
@@ -41668,7 +41658,7 @@
         <v>22</v>
       </c>
       <c r="F664" s="9" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G664" s="9" t="s">
         <v>23</v>
@@ -41786,7 +41776,7 @@
         <v>22</v>
       </c>
       <c r="F666" s="9" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="G666" s="9" t="s">
         <v>23</v>
@@ -42140,7 +42130,7 @@
         <v>22</v>
       </c>
       <c r="F672" s="9" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="G672" s="9" t="s">
         <v>23</v>
@@ -42612,7 +42602,7 @@
         <v>22</v>
       </c>
       <c r="F680" s="9" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="G680" s="9" t="s">
         <v>23</v>
@@ -42850,7 +42840,7 @@
         <v>22</v>
       </c>
       <c r="F684" s="9" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="G684" s="9" t="s">
         <v>23</v>
@@ -42970,7 +42960,7 @@
         <v>22</v>
       </c>
       <c r="F686" s="9" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="G686" s="9" t="s">
         <v>23</v>
@@ -43147,7 +43137,7 @@
         <v>22</v>
       </c>
       <c r="F689" s="9" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="G689" s="9" t="s">
         <v>23</v>
@@ -43737,7 +43727,7 @@
         <v>22</v>
       </c>
       <c r="F699" s="9" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="G699" s="9" t="s">
         <v>23</v>
@@ -44091,7 +44081,7 @@
         <v>22</v>
       </c>
       <c r="F705" s="9" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="G705" s="9" t="s">
         <v>23</v>
@@ -44386,7 +44376,7 @@
         <v>22</v>
       </c>
       <c r="F710" s="9" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="G710" s="9" t="s">
         <v>23</v>
@@ -44504,7 +44494,7 @@
         <v>22</v>
       </c>
       <c r="F712" s="9" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G712" s="9" t="s">
         <v>23</v>
@@ -44681,7 +44671,7 @@
         <v>22</v>
       </c>
       <c r="F715" s="9" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="G715" s="9" t="s">
         <v>23</v>
@@ -44858,7 +44848,7 @@
         <v>22</v>
       </c>
       <c r="F718" s="9" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="G718" s="9" t="s">
         <v>23</v>
@@ -45155,7 +45145,7 @@
         <v>22</v>
       </c>
       <c r="F723" s="9" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G723" s="9" t="s">
         <v>23</v>
@@ -45450,7 +45440,7 @@
         <v>22</v>
       </c>
       <c r="F728" s="9" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="G728" s="9" t="s">
         <v>23</v>
@@ -45686,7 +45676,7 @@
         <v>22</v>
       </c>
       <c r="F732" s="9" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="G732" s="9" t="s">
         <v>23</v>
@@ -45745,7 +45735,7 @@
         <v>22</v>
       </c>
       <c r="F733" s="9" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="G733" s="9" t="s">
         <v>23</v>
@@ -45922,7 +45912,7 @@
         <v>22</v>
       </c>
       <c r="F736" s="9" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="G736" s="9" t="s">
         <v>23</v>
@@ -46022,7 +46012,7 @@
         <v>99880</v>
       </c>
       <c r="U737" s="8" t="s">
-        <v>138</v>
+        <v>611</v>
       </c>
     </row>
     <row r="738" spans="1:21">
@@ -46042,7 +46032,7 @@
         <v>22</v>
       </c>
       <c r="F738" s="9" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="G738" s="9" t="s">
         <v>23</v>
@@ -46101,7 +46091,7 @@
         <v>22</v>
       </c>
       <c r="F739" s="9" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="G739" s="9" t="s">
         <v>23</v>
@@ -46219,7 +46209,7 @@
         <v>22</v>
       </c>
       <c r="F741" s="9" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="G741" s="9" t="s">
         <v>23</v>
@@ -46278,7 +46268,7 @@
         <v>22</v>
       </c>
       <c r="F742" s="9" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="G742" s="9" t="s">
         <v>23</v>
@@ -46396,7 +46386,7 @@
         <v>22</v>
       </c>
       <c r="F744" s="9" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="G744" s="9" t="s">
         <v>23</v>
@@ -47224,7 +47214,7 @@
         <v>22</v>
       </c>
       <c r="F758" s="9" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="G758" s="9" t="s">
         <v>23</v>
@@ -48113,7 +48103,7 @@
         <v>22</v>
       </c>
       <c r="F773" s="9" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="G773" s="9" t="s">
         <v>23</v>
@@ -48211,7 +48201,7 @@
         <v>300</v>
       </c>
       <c r="U774" s="8" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="775" spans="1:21">
@@ -48469,7 +48459,7 @@
         <v>22</v>
       </c>
       <c r="F779" s="9" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="G779" s="9" t="s">
         <v>23</v>
@@ -48646,7 +48636,7 @@
         <v>22</v>
       </c>
       <c r="F782" s="9" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="G782" s="9" t="s">
         <v>23</v>
@@ -49000,7 +48990,7 @@
         <v>22</v>
       </c>
       <c r="F788" s="9" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="G788" s="9" t="s">
         <v>23</v>
@@ -49354,7 +49344,7 @@
         <v>22</v>
       </c>
       <c r="F794" s="9" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G794" s="9" t="s">
         <v>23</v>
@@ -49472,7 +49462,7 @@
         <v>22</v>
       </c>
       <c r="F796" s="9" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="G796" s="9" t="s">
         <v>23</v>
@@ -49531,7 +49521,7 @@
         <v>22</v>
       </c>
       <c r="F797" s="9" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="G797" s="9" t="s">
         <v>23</v>
@@ -49649,7 +49639,7 @@
         <v>22</v>
       </c>
       <c r="F799" s="9" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="G799" s="9" t="s">
         <v>23</v>
@@ -49944,7 +49934,7 @@
         <v>22</v>
       </c>
       <c r="F804" s="9" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="G804" s="9" t="s">
         <v>23</v>
@@ -50182,7 +50172,7 @@
         <v>22</v>
       </c>
       <c r="F808" s="9" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="G808" s="9" t="s">
         <v>23</v>
@@ -50418,7 +50408,7 @@
         <v>22</v>
       </c>
       <c r="F812" s="9" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="G812" s="9" t="s">
         <v>23</v>
@@ -50477,7 +50467,7 @@
         <v>22</v>
       </c>
       <c r="F813" s="9" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="G813" s="9" t="s">
         <v>23</v>
@@ -50536,7 +50526,7 @@
         <v>22</v>
       </c>
       <c r="F814" s="9" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="G814" s="9" t="s">
         <v>23</v>
@@ -50637,7 +50627,7 @@
         <v>0</v>
       </c>
       <c r="U815" s="8" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="816" spans="1:21" ht="26">
@@ -50699,7 +50689,7 @@
         <v>0</v>
       </c>
       <c r="U816" s="8" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="817" spans="1:21" ht="26">
@@ -50956,7 +50946,7 @@
         <v>22</v>
       </c>
       <c r="F821" s="9" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="G821" s="9" t="s">
         <v>23</v>
@@ -51133,7 +51123,7 @@
         <v>22</v>
       </c>
       <c r="F824" s="9" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="G824" s="9" t="s">
         <v>23</v>
@@ -51192,13 +51182,13 @@
         <v>22</v>
       </c>
       <c r="F825" s="9" t="s">
+        <v>572</v>
+      </c>
+      <c r="G825" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H825" s="19" t="s">
         <v>573</v>
-      </c>
-      <c r="G825" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H825" s="19" t="s">
-        <v>574</v>
       </c>
       <c r="I825" s="11">
         <v>11667</v>
@@ -51257,7 +51247,7 @@
         <v>23</v>
       </c>
       <c r="H826" s="19" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I826" s="11">
         <v>13400</v>
@@ -51316,7 +51306,7 @@
         <v>23</v>
       </c>
       <c r="H827" s="19" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I827" s="11">
         <v>503251</v>
@@ -51375,7 +51365,7 @@
         <v>23</v>
       </c>
       <c r="H828" s="19" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I828" s="11">
         <v>77375</v>
@@ -51434,7 +51424,7 @@
         <v>23</v>
       </c>
       <c r="H829" s="19" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I829" s="11">
         <v>125</v>
@@ -51493,7 +51483,7 @@
         <v>23</v>
       </c>
       <c r="H830" s="19" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I830" s="11">
         <v>589857</v>
@@ -51552,7 +51542,7 @@
         <v>23</v>
       </c>
       <c r="H831" s="19" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I831" s="11">
         <v>1981033</v>
@@ -51611,7 +51601,7 @@
         <v>23</v>
       </c>
       <c r="H832" s="19" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I832" s="11">
         <v>104988</v>
@@ -51670,7 +51660,7 @@
         <v>23</v>
       </c>
       <c r="H833" s="19" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I833" s="11">
         <v>5172</v>
@@ -51723,13 +51713,13 @@
         <v>22</v>
       </c>
       <c r="F834" s="18" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="G834" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H834" s="19" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I834" s="11">
         <v>308</v>
@@ -51788,7 +51778,7 @@
         <v>23</v>
       </c>
       <c r="H835" s="19" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I835" s="11">
         <v>23483</v>
@@ -51841,13 +51831,13 @@
         <v>22</v>
       </c>
       <c r="F836" s="9" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="G836" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H836" s="19" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I836" s="11">
         <v>211241</v>
@@ -51906,7 +51896,7 @@
         <v>23</v>
       </c>
       <c r="H837" s="19" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I837" s="11">
         <v>1524</v>
@@ -51959,13 +51949,13 @@
         <v>22</v>
       </c>
       <c r="F838" s="9" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="G838" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H838" s="19" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I838" s="11">
         <v>728</v>
@@ -52024,7 +52014,7 @@
         <v>23</v>
       </c>
       <c r="H839" s="19" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I839" s="11">
         <v>150292</v>
@@ -52077,13 +52067,13 @@
         <v>22</v>
       </c>
       <c r="F840" s="9" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="G840" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H840" s="19" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I840" s="11">
         <v>715</v>
@@ -52136,13 +52126,13 @@
         <v>22</v>
       </c>
       <c r="F841" s="9" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="G841" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H841" s="19" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I841" s="11">
         <v>25</v>
@@ -52201,7 +52191,7 @@
         <v>23</v>
       </c>
       <c r="H842" s="19" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I842" s="11">
         <v>1958</v>
@@ -52260,7 +52250,7 @@
         <v>23</v>
       </c>
       <c r="H843" s="19" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I843" s="11">
         <v>150214</v>
@@ -52319,7 +52309,7 @@
         <v>23</v>
       </c>
       <c r="H844" s="19" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I844" s="11">
         <v>109</v>
@@ -52378,7 +52368,7 @@
         <v>23</v>
       </c>
       <c r="H845" s="19" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I845" s="11">
         <v>1805475</v>
@@ -52437,7 +52427,7 @@
         <v>23</v>
       </c>
       <c r="H846" s="19" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I846" s="11">
         <v>13312995</v>
@@ -52496,7 +52486,7 @@
         <v>23</v>
       </c>
       <c r="H847" s="19" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I847" s="11">
         <v>1834658</v>
@@ -52549,13 +52539,13 @@
         <v>22</v>
       </c>
       <c r="F848" s="9" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="G848" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H848" s="19" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I848" s="11">
         <v>1497</v>
@@ -52608,13 +52598,13 @@
         <v>22</v>
       </c>
       <c r="F849" s="9" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="G849" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H849" s="19" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I849" s="11">
         <v>313</v>
@@ -52673,7 +52663,7 @@
         <v>23</v>
       </c>
       <c r="H850" s="19" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I850" s="11">
         <f>80+(13/16)</f>

</xml_diff>